<commit_message>
added test cases for data driven testing
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TejashwaRajvardhan\IdeaProjects\OpenCartv0.4\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C1ADBA-0BA8-4A24-B1A6-553D88F004CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E1BCF2-F228-4E49-B7E4-C1E4ECECF8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7A6ED804-763A-4955-A476-CF4D69A30691}"/>
   </bookViews>
@@ -163,7 +163,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>